<commit_message>
join 2 dataTable dan membandingkat kedua data table tsb
</commit_message>
<xml_diff>
--- a/DataReconciliation/Data/VendorData.xlsx
+++ b/DataReconciliation/Data/VendorData.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1458\Documents\UiPath\DataReconciliation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1458\Documents\UiPath\Uipath-journey\DataReconciliation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8825B268-98FC-4E63-BB11-D091015716A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92690D71-BEF0-4164-B02B-DDF560D48C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -381,9 +381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>